<commit_message>
se suben ajustes para los portin
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla2\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA1ECCE-F388-4EE7-9C15-943681FC0692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C594B135-6A11-4F77-98B6-E97844B28B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="95">
   <si>
     <t>MSIDN</t>
   </si>
@@ -299,6 +299,18 @@
   </si>
   <si>
     <t>732111324706350</t>
+  </si>
+  <si>
+    <t>69883703</t>
+  </si>
+  <si>
+    <t>345769284</t>
+  </si>
+  <si>
+    <t>3045984556</t>
+  </si>
+  <si>
+    <t>732111193278721</t>
   </si>
 </sst>
 </file>
@@ -387,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -412,6 +424,7 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -729,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -740,10 +753,11 @@
     <col min="3" max="3" width="24.5703125" style="11" customWidth="1"/>
     <col min="4" max="4" width="31.140625" style="11" customWidth="1"/>
     <col min="5" max="5" width="30.85546875" style="11" customWidth="1"/>
-    <col min="6" max="16384" width="11.42578125" style="11"/>
+    <col min="6" max="6" width="19" style="11" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="12" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -772,7 +786,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1">
+    <row r="2" spans="1:9" s="12" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -797,11 +811,11 @@
       <c r="H2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1">
+    <row r="3" spans="1:9" s="12" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -814,8 +828,13 @@
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" s="12" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>74</v>
       </c>
@@ -837,8 +856,10 @@
       <c r="G4" s="8" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" s="12" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>76</v>
       </c>
@@ -860,8 +881,10 @@
       <c r="G5" s="9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" s="12" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>76</v>
       </c>
@@ -874,8 +897,13 @@
       <c r="D6" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" s="12" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -888,8 +916,13 @@
       <c r="D7" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" s="12" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -918,7 +951,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1">
+    <row r="9" spans="1:9" s="12" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -932,22 +965,22 @@
         <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>39</v>
+        <v>93</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="1">
-        <v>411661795</v>
+      <c r="H9" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1">
+    <row r="10" spans="1:9" s="12" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
@@ -969,14 +1002,14 @@
       <c r="G10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="1">
-        <v>582710820</v>
+      <c r="H10" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1">
+    <row r="11" spans="1:9" s="12" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -989,8 +1022,13 @@
       <c r="D11" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" s="12" customFormat="1">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -1003,8 +1041,13 @@
       <c r="D12" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" s="12" customFormat="1">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1017,8 +1060,13 @@
       <c r="D13" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" customFormat="1">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1031,6 +1079,11 @@
       <c r="D14" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
se suben ajustes para port in
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla2\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C594B135-6A11-4F77-98B6-E97844B28B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFB790A-9871-4A0A-98C6-5780160565DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,43 +274,43 @@
     <t>3046008593</t>
   </si>
   <si>
+    <t>582710820</t>
+  </si>
+  <si>
+    <t>477140225</t>
+  </si>
+  <si>
+    <t>261605166</t>
+  </si>
+  <si>
+    <t>188145974</t>
+  </si>
+  <si>
+    <t>732111193280551</t>
+  </si>
+  <si>
+    <t>732111193280544</t>
+  </si>
+  <si>
+    <t>732111193280535</t>
+  </si>
+  <si>
+    <t>69883703</t>
+  </si>
+  <si>
+    <t>345769284</t>
+  </si>
+  <si>
+    <t>732111193278721</t>
+  </si>
+  <si>
     <t>3043118820</t>
   </si>
   <si>
-    <t>582710820</t>
-  </si>
-  <si>
-    <t>477140225</t>
-  </si>
-  <si>
-    <t>261605166</t>
-  </si>
-  <si>
-    <t>188145974</t>
-  </si>
-  <si>
-    <t>732111193280551</t>
-  </si>
-  <si>
-    <t>732111193280544</t>
-  </si>
-  <si>
-    <t>732111193280535</t>
-  </si>
-  <si>
     <t>732111324706350</t>
   </si>
   <si>
-    <t>69883703</t>
-  </si>
-  <si>
-    <t>345769284</t>
-  </si>
-  <si>
     <t>3045984556</t>
-  </si>
-  <si>
-    <t>732111193278721</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -424,7 +424,9 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -742,22 +744,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="19" style="11" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="11"/>
+    <col min="1" max="1" width="26.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="19" style="13" customWidth="1"/>
+    <col min="7" max="16384" width="11.42578125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="12" customFormat="1">
+    <row r="1" spans="1:9" s="14" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -786,7 +788,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="12" customFormat="1">
+    <row r="2" spans="1:9" s="14" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>71</v>
       </c>
@@ -815,7 +817,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="12" customFormat="1">
+    <row r="3" spans="1:9" s="14" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -834,7 +836,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" s="12" customFormat="1">
+    <row r="4" spans="1:9" s="14" customFormat="1">
       <c r="A4" s="5" t="s">
         <v>74</v>
       </c>
@@ -859,7 +861,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" s="12" customFormat="1">
+    <row r="5" spans="1:9" s="14" customFormat="1">
       <c r="A5" s="5" t="s">
         <v>76</v>
       </c>
@@ -884,7 +886,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" s="12" customFormat="1">
+    <row r="6" spans="1:9" s="14" customFormat="1">
       <c r="A6" s="5" t="s">
         <v>76</v>
       </c>
@@ -903,7 +905,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" s="12" customFormat="1">
+    <row r="7" spans="1:9" s="14" customFormat="1">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -922,7 +924,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" s="12" customFormat="1">
+    <row r="8" spans="1:9" s="14" customFormat="1">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -951,50 +953,50 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="12" customFormat="1">
+    <row r="9" spans="1:9" s="14" customFormat="1">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>78</v>
+        <v>82</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>44</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="12" customFormat="1">
+    <row r="10" spans="1:9" s="14" customFormat="1">
       <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>79</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>54</v>
@@ -1003,87 +1005,87 @@
         <v>45</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="12" customFormat="1">
+    <row r="11" spans="1:9" s="14" customFormat="1">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" s="12" customFormat="1">
+        <v>93</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" s="14" customFormat="1">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" s="12" customFormat="1">
+        <v>87</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="1:9" s="14" customFormat="1">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>81</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
+        <v>88</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Se realizan cambios para portInPrepago
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla2\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\SanitySemillas\SanitySemilla2\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229562FA-CB01-4069-9635-2F66D462C17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F94156-877F-4456-B31A-4A903B34461F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 2" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
   <si>
     <t>MSIDN</t>
   </si>
@@ -289,9 +289,6 @@
     <t>345769284</t>
   </si>
   <si>
-    <t>732111193278721</t>
-  </si>
-  <si>
     <t>3045984556</t>
   </si>
   <si>
@@ -307,16 +304,22 @@
     <t>732111193278863</t>
   </si>
   <si>
+    <t>199851863</t>
+  </si>
+  <si>
+    <t>663573097</t>
+  </si>
+  <si>
+    <t>3043118820</t>
+  </si>
+  <si>
+    <t>732111324706350</t>
+  </si>
+  <si>
     <t>3045987650</t>
   </si>
   <si>
     <t>732111193278858</t>
-  </si>
-  <si>
-    <t>199851863</t>
-  </si>
-  <si>
-    <t>663573097</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D18:D19"/>
+      <selection activeCell="C9" sqref="C9:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -970,16 +973,16 @@
         <v>80</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>44</v>
@@ -997,13 +1000,13 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>79</v>
@@ -1030,10 +1033,10 @@
         <v>80</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -1049,11 +1052,11 @@
       <c r="B12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>94</v>
+      <c r="C12" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -1087,10 +1090,10 @@
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>84</v>
@@ -1102,7 +1105,7 @@
       <c r="I14" s="10"/>
       <c r="J14"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
se agrea clase TestLinkIntegration.java y se implementa el metodo para actualizar el caso en testlink
</commit_message>
<xml_diff>
--- a/build/resources/test/config_data/data.xlsx
+++ b/build/resources/test/config_data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nriosa\Desktop\SanitySemillas\SanitySemilla2\src\test\resources\config_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SanitySemilla2\src\test\resources\config_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F94156-877F-4456-B31A-4A903B34461F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10771547-CBF7-499B-BA1D-B728BE155CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semilla 2" sheetId="2" r:id="rId1"/>
@@ -304,22 +304,22 @@
     <t>732111193278863</t>
   </si>
   <si>
+    <t>3045987650</t>
+  </si>
+  <si>
+    <t>732111193278858</t>
+  </si>
+  <si>
     <t>199851863</t>
   </si>
   <si>
     <t>663573097</t>
   </si>
   <si>
+    <t>732111324706350</t>
+  </si>
+  <si>
     <t>3043118820</t>
-  </si>
-  <si>
-    <t>732111324706350</t>
-  </si>
-  <si>
-    <t>3045987650</t>
-  </si>
-  <si>
-    <t>732111193278858</t>
   </si>
 </sst>
 </file>
@@ -756,7 +756,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:D15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -979,10 +979,10 @@
         <v>89</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>44</v>
@@ -1000,7 +1000,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>90</v>
@@ -1052,11 +1052,11 @@
       <c r="B12" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" s="14" t="s">
+      <c r="C12" s="1" t="s">
         <v>97</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
@@ -1090,7 +1090,7 @@
         <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>87</v>
@@ -1105,7 +1105,7 @@
       <c r="I14" s="10"/>
       <c r="J14"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -1130,6 +1130,9 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
+  <ignoredErrors>
+    <ignoredError sqref="D12" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>